<commit_message>
adding grib to webpages
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom_all.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom_all.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386E7809-B794-DF4B-9719-1DC7982E3078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76EE113-E9AE-704C-87DC-DDFC81D774F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Station ID</t>
   </si>
@@ -219,19 +219,22 @@
     <t>Row Label</t>
   </si>
   <si>
+    <t>Custer Arpt, SD</t>
+  </si>
+  <si>
     <t>Ellsworth AFB, SD</t>
   </si>
   <si>
+    <t>Hulett Arpt, WY</t>
+  </si>
+  <si>
     <t>Pine Ridge Arpt, SD</t>
   </si>
   <si>
-    <t>Custer Arpt, SD</t>
-  </si>
-  <si>
-    <t>Hulett Arpt, WY</t>
-  </si>
-  <si>
     <t>Philip Arpt, SD</t>
+  </si>
+  <si>
+    <t>Distane from UNR</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -290,17 +293,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -615,9 +632,10 @@
     <col min="1" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="6" width="30.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -636,48 +654,57 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E2">
-        <v>43.732999999999997</v>
+        <v>44.072699999999998</v>
       </c>
       <c r="F2">
-        <v>-103.611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-103.211</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="E3">
-        <v>44.734000000000002</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F3">
-        <v>-103.86199999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-103.1</v>
+      </c>
+      <c r="G3">
+        <v>1.5957090000001551E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -696,328 +723,379 @@
       <c r="F4">
         <v>-103.054</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>2.5531089999998792E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>44.133000000000003</v>
       </c>
       <c r="F5">
-        <v>-103.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-102.833</v>
+      </c>
+      <c r="G5">
+        <v>0.14652009000000071</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>43.732999999999997</v>
+      </c>
+      <c r="F6">
+        <v>-103.611</v>
+      </c>
+      <c r="G6">
+        <v>0.27539609000000492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>44.482999999999997</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>-103.783</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7">
-        <v>44.133000000000003</v>
-      </c>
-      <c r="F7">
-        <v>-102.833</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0.4955300900000027</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>44.734000000000002</v>
+      </c>
+      <c r="F8">
+        <v>-103.86199999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.86111869000000074</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>42.837000000000003</v>
+      </c>
+      <c r="F9">
+        <v>-103.098</v>
+      </c>
+      <c r="G9">
+        <v>1.5397234899999857</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10">
+        <v>43.021000000000001</v>
+      </c>
+      <c r="F10">
+        <v>-102.518</v>
+      </c>
+      <c r="G10">
+        <v>1.5863218899999902</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>44.6629</v>
+      </c>
+      <c r="F11">
+        <v>-104.568</v>
+      </c>
+      <c r="G11">
+        <v>2.1897850400000016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12">
+        <v>45.031999999999996</v>
+      </c>
+      <c r="F12">
+        <v>-102.01900000000001</v>
+      </c>
+      <c r="G12">
+        <v>2.3411204899999816</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <v>45.603999999999999</v>
+      </c>
+      <c r="F13">
+        <v>-103.54600000000001</v>
+      </c>
+      <c r="G13">
+        <v>2.4571046900000106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14">
+        <v>44.051000000000002</v>
+      </c>
+      <c r="F14">
+        <v>-101.601</v>
+      </c>
+      <c r="G14">
+        <v>2.592570889999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>42.805999999999997</v>
+      </c>
+      <c r="F15">
+        <v>-102.175</v>
+      </c>
+      <c r="G15">
+        <v>2.6778248900000032</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>44.267000000000003</v>
+      </c>
+      <c r="F16">
+        <v>-104.95</v>
+      </c>
+      <c r="G16">
+        <v>3.0618734900000173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17">
+        <v>46.017000000000003</v>
+      </c>
+      <c r="F17">
+        <v>-102.65</v>
+      </c>
+      <c r="G17">
+        <v>4.0950234900000133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18">
+        <v>42.05</v>
+      </c>
+      <c r="F18">
+        <v>-102.8</v>
+      </c>
+      <c r="G18">
+        <v>4.2602362900000026</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>46.186999999999998</v>
+      </c>
+      <c r="F19">
+        <v>-103.428</v>
+      </c>
+      <c r="G19">
+        <v>4.5173534899999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8">
-        <v>44.072699999999998</v>
-      </c>
-      <c r="F8">
-        <v>-103.211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9">
-        <v>44.6629</v>
-      </c>
-      <c r="F9">
-        <v>-104.568</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10">
-        <v>45.603999999999999</v>
-      </c>
-      <c r="F10">
-        <v>-103.54600000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11">
-        <v>42.75</v>
-      </c>
-      <c r="F11">
-        <v>-105.383</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12">
-        <v>44.267000000000003</v>
-      </c>
-      <c r="F12">
-        <v>-104.95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13">
-        <v>46.186999999999998</v>
-      </c>
-      <c r="F13">
-        <v>-103.428</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14">
-        <v>42.837000000000003</v>
-      </c>
-      <c r="F14">
-        <v>-103.098</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15">
-        <v>45.031999999999996</v>
-      </c>
-      <c r="F15">
-        <v>-102.01900000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16">
-        <v>42.795999999999999</v>
-      </c>
-      <c r="F16">
-        <v>-105.38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17">
-        <v>44.338999999999999</v>
-      </c>
-      <c r="F17">
-        <v>-105.542</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18">
-        <v>42.805999999999997</v>
-      </c>
-      <c r="F18">
-        <v>-102.175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19">
-        <v>46.017000000000003</v>
-      </c>
-      <c r="F19">
-        <v>-102.65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E20">
-        <v>43.021000000000001</v>
+        <v>45.933</v>
       </c>
       <c r="F20">
-        <v>-102.518</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-102.167</v>
+      </c>
+      <c r="G20">
+        <v>4.5506520900000016</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1036,188 +1114,218 @@
       <c r="F21">
         <v>-102.10599999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>4.6298486900000064</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22">
+        <v>42.061</v>
+      </c>
+      <c r="F22">
+        <v>-104.158</v>
+      </c>
+      <c r="G22">
+        <v>4.9437458899999962</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>41.871000000000002</v>
+      </c>
+      <c r="F23">
+        <v>-103.593</v>
+      </c>
+      <c r="G23">
+        <v>4.9934068899999833</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24">
+        <v>44.338999999999999</v>
+      </c>
+      <c r="F24">
+        <v>-105.542</v>
+      </c>
+      <c r="G24">
+        <v>5.5044766900000148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25">
+        <v>42.433</v>
+      </c>
+      <c r="F25">
+        <v>-105.033</v>
+      </c>
+      <c r="G25">
+        <v>6.0083000900000023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>42.795999999999999</v>
+      </c>
+      <c r="F26">
+        <v>-105.38</v>
+      </c>
+      <c r="G26">
+        <v>6.3345238899999821</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27">
+        <v>42.75</v>
+      </c>
+      <c r="F27">
+        <v>-105.383</v>
+      </c>
+      <c r="G27">
+        <v>6.4671192899999808</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E22">
+      <c r="E28">
         <v>43.033000000000001</v>
       </c>
-      <c r="F22">
+      <c r="F28">
         <v>-100.617</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23">
-        <v>44.051000000000002</v>
-      </c>
-      <c r="F23">
-        <v>-101.601</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="G28">
+        <v>7.8098120899999612</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29">
+        <v>42.878</v>
+      </c>
+      <c r="F29">
+        <v>-100.55</v>
+      </c>
+      <c r="G29">
+        <v>8.5082290900000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>19</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B30" t="s">
         <v>24</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E24">
+      <c r="E30">
         <v>44.381</v>
       </c>
-      <c r="F24">
+      <c r="F30">
         <v>-100.286</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>27</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25">
-        <v>42.878</v>
-      </c>
-      <c r="F25">
-        <v>-100.55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26">
-        <v>45.933</v>
-      </c>
-      <c r="F26">
-        <v>-102.167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27">
-        <v>42.05</v>
-      </c>
-      <c r="F27">
-        <v>-102.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>4</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28">
-        <v>41.871000000000002</v>
-      </c>
-      <c r="F28">
-        <v>-103.593</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29">
-        <v>42.433</v>
-      </c>
-      <c r="F29">
-        <v>-105.033</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30">
-        <v>42.061</v>
-      </c>
-      <c r="F30">
-        <v>-104.158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>8.6506738899999842</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1236,11 +1344,14 @@
       <c r="F31">
         <v>-98.834999999999994</v>
       </c>
+      <c r="G31">
+        <v>40.254212000000102</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
-      <sortCondition descending="1" ref="C1:C32"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
+      <sortCondition ref="G1:G31"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updating bowman airport bww location.
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom_all.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39679ED-FD20-4E4E-8B07-C809EA8F2DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13434DE4-B9FA-DB44-8861-A87E7C5F118A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-340" yWindow="2240" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>K4MC</t>
   </si>
   <si>
-    <t>KBPP</t>
-  </si>
-  <si>
     <t>KCDR</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Distane from SDMines</t>
+  </si>
+  <si>
+    <t>KBWW</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -683,13 +683,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="3">
         <v>44.072699999999998</v>
@@ -706,13 +706,13 @@
         <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="3">
         <v>44.133000000000003</v>
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3">
         <v>44.042999999999999</v>
@@ -752,13 +752,13 @@
         <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3">
         <v>44.133000000000003</v>
@@ -775,13 +775,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="3">
         <v>43.732999999999997</v>
@@ -798,13 +798,13 @@
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="3">
         <v>44.482999999999997</v>
@@ -821,13 +821,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="3">
         <v>44.734000000000002</v>
@@ -844,13 +844,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3">
         <v>42.837000000000003</v>
@@ -867,13 +867,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3">
         <v>43.021000000000001</v>
@@ -890,13 +890,13 @@
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3">
         <v>44.6629</v>
@@ -913,13 +913,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3">
         <v>45.031999999999996</v>
@@ -942,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="3">
         <v>45.603999999999999</v>
@@ -959,13 +959,13 @@
         <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3">
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="3">
         <v>44.051000000000002</v>
@@ -982,13 +982,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3">
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="3">
         <v>42.805999999999997</v>
@@ -1011,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="3">
         <v>44.267000000000003</v>
@@ -1028,13 +1028,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3">
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="3">
         <v>46.017000000000003</v>
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3">
         <v>42.05</v>
@@ -1074,19 +1074,19 @@
         <v>5</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3">
         <v>2</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="3">
-        <v>46.186999999999998</v>
+        <v>46.165500000000002</v>
       </c>
       <c r="F19" s="3">
-        <v>-103.428</v>
+        <v>-103.3</v>
       </c>
       <c r="G19" s="5">
         <v>235.57785564806699</v>
@@ -1097,13 +1097,13 @@
         <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3">
         <v>45.933</v>
@@ -1120,13 +1120,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="3">
         <v>45.918999999999997</v>
@@ -1149,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="3">
         <v>42.061</v>
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3">
         <v>41.871000000000002</v>
@@ -1189,13 +1189,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="3">
         <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="3">
         <v>44.338999999999999</v>
@@ -1218,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="3">
         <v>42.433</v>
@@ -1235,13 +1235,13 @@
         <v>9</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="3">
         <v>2</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="3">
         <v>42.795999999999999</v>
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="3">
         <v>42.75</v>
@@ -1281,13 +1281,13 @@
         <v>17</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="3">
         <v>2</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="3">
         <v>43.033000000000001</v>
@@ -1304,13 +1304,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3">
         <v>2</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29" s="3">
         <v>42.878</v>
@@ -1327,13 +1327,13 @@
         <v>19</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="3">
         <v>2</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="3">
         <v>44.381</v>
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E31" s="3">
         <v>48.666699999999999</v>

</xml_diff>

<commit_message>
adding stations to html files
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom_all.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom_all.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8411D339-7AEB-1145-BDE1-DF6C96921D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB828546-685F-BF41-8B27-78B2807CC4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="1080" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="1020" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,280 +56,280 @@
     <t>KUNR</t>
   </si>
   <si>
-    <t>RAPID CITY NWS SD</t>
-  </si>
-  <si>
     <t>KRCA</t>
   </si>
   <si>
-    <t>ELLSWORTH AFB SD</t>
-  </si>
-  <si>
     <t>KRAP</t>
   </si>
   <si>
-    <t>RAPID CITY ARPT SD</t>
-  </si>
-  <si>
     <t>KUDX</t>
   </si>
   <si>
-    <t>RAPID CITY NEXRAD SD</t>
-  </si>
-  <si>
     <t>KCUT</t>
   </si>
   <si>
-    <t>CUSTER AIRPORT SD</t>
-  </si>
-  <si>
     <t>KSPF</t>
   </si>
   <si>
-    <t>CLYDE ICE FIELD SD</t>
-  </si>
-  <si>
     <t>KEFC</t>
   </si>
   <si>
-    <t>BELLE FOURCHE MUNI SD</t>
-  </si>
-  <si>
     <t>KW43</t>
   </si>
   <si>
-    <t>HULETT AIRPORT WY</t>
-  </si>
-  <si>
     <t>KPHP</t>
   </si>
   <si>
-    <t>PHILIP AIRPORT SD</t>
-  </si>
-  <si>
     <t>KIEN</t>
   </si>
   <si>
-    <t>PINE RIDGE AIRPORT SD</t>
-  </si>
-  <si>
     <t>KCDR</t>
   </si>
   <si>
-    <t>CHADRON AIRPORT NE</t>
-  </si>
-  <si>
     <t>K4MC</t>
   </si>
   <si>
-    <t>MOORCROFT WY</t>
-  </si>
-  <si>
     <t>KD07</t>
   </si>
   <si>
-    <t>FAITH AIRPORT SD</t>
-  </si>
-  <si>
     <t>KGRN</t>
   </si>
   <si>
-    <t>GORDON MUNI NE</t>
-  </si>
-  <si>
     <t>K2WX</t>
   </si>
   <si>
-    <t>BUFFALO SD</t>
-  </si>
-  <si>
     <t>KGCC</t>
   </si>
   <si>
-    <t>GILLETTE  ARPT WY</t>
-  </si>
-  <si>
     <t>KHEI</t>
   </si>
   <si>
-    <t>HETTINGER ARPT ND</t>
-  </si>
-  <si>
     <t>KY22</t>
   </si>
   <si>
-    <t>LEMMON SD</t>
-  </si>
-  <si>
     <t>KLEM</t>
   </si>
   <si>
-    <t>LEMMON ARPT SD</t>
-  </si>
-  <si>
     <t>KDGW</t>
   </si>
   <si>
-    <t>CONVERSE CO ARPT WY</t>
-  </si>
-  <si>
     <t>KAIA</t>
   </si>
   <si>
-    <t>ALLIANCE ARPT NE</t>
-  </si>
-  <si>
     <t>K4DG</t>
   </si>
   <si>
-    <t>DOUGLAS WY</t>
-  </si>
-  <si>
     <t>KBWW</t>
   </si>
   <si>
-    <t>BOWMAN ARPT ND</t>
-  </si>
-  <si>
     <t>KSIB</t>
   </si>
   <si>
-    <t>SIBLEY PEAK WY</t>
-  </si>
-  <si>
     <t>KPIR</t>
   </si>
   <si>
-    <t>PIERRE ARPT SD</t>
-  </si>
-  <si>
     <t>KTOR</t>
   </si>
   <si>
-    <t>TORRINGTON ARPT WY</t>
-  </si>
-  <si>
     <t>KMIS</t>
   </si>
   <si>
-    <t>MISSION SD</t>
-  </si>
-  <si>
     <t>KBFF</t>
   </si>
   <si>
-    <t>SCOTTSBLUFF ARPT NE</t>
-  </si>
-  <si>
     <t>KVTN</t>
   </si>
   <si>
-    <t>MILLER FIELD ARPT NE</t>
-  </si>
-  <si>
     <t>KCYS</t>
   </si>
   <si>
-    <t>CHEYENNE NWS WY</t>
-  </si>
-  <si>
     <t>KBIS</t>
   </si>
   <si>
-    <t>BISMARK NWS ND</t>
-  </si>
-  <si>
     <t>KLBF</t>
   </si>
   <si>
-    <t>NORTH PLATTE NWS NE</t>
-  </si>
-  <si>
     <t>KABR</t>
   </si>
   <si>
-    <t>ABERDEEN NWS SD</t>
-  </si>
-  <si>
     <t>KRIW</t>
   </si>
   <si>
-    <t>RIVERTON NWS WY</t>
-  </si>
-  <si>
     <t>KBYZ</t>
   </si>
   <si>
-    <t>BILLINGS NWS MT</t>
-  </si>
-  <si>
     <t>KDEN</t>
   </si>
   <si>
-    <t>DENVER INTL AIRPORT CO</t>
-  </si>
-  <si>
     <t>KBOU</t>
   </si>
   <si>
-    <t>BOULDER NWS CO</t>
-  </si>
-  <si>
     <t>KFSD</t>
   </si>
   <si>
-    <t>SIOUX FALLS NWS SD</t>
-  </si>
-  <si>
     <t>KGGW</t>
   </si>
   <si>
-    <t>GLASGOW NWS MT</t>
-  </si>
-  <si>
     <t>KGLD</t>
   </si>
   <si>
-    <t>GOODLAND NWS KS</t>
-  </si>
-  <si>
     <t>KGID</t>
   </si>
   <si>
-    <t>HASTINGS NWS NE</t>
-  </si>
-  <si>
     <t>MUNS</t>
   </si>
   <si>
-    <t>MUNICH SCHOOL ND</t>
-  </si>
-  <si>
     <t>KFGF</t>
   </si>
   <si>
-    <t>GRAND FORKS NWS ND</t>
-  </si>
-  <si>
     <t>KOAX</t>
   </si>
   <si>
-    <t>OMAHA-VALLEY NWS NE</t>
-  </si>
-  <si>
     <t>KGJT</t>
   </si>
   <si>
-    <t>GRAND JUNCTION NWS CO</t>
-  </si>
-  <si>
     <t>KTOP</t>
   </si>
   <si>
-    <t>TOPEKA NWS KS</t>
-  </si>
-  <si>
     <t>Row Label</t>
+  </si>
+  <si>
+    <t>Rapid City NWS, SD</t>
+  </si>
+  <si>
+    <t>Ellsworth AFB, SD</t>
+  </si>
+  <si>
+    <t>Rapid City Airport, SD</t>
+  </si>
+  <si>
+    <t>Rapid City, NEXRAD, SD</t>
+  </si>
+  <si>
+    <t>Custer Airport, SD</t>
+  </si>
+  <si>
+    <t>Clyde Ice Field, SD</t>
+  </si>
+  <si>
+    <t>Belle Fourche Airport, SD</t>
+  </si>
+  <si>
+    <t>Hulett Airport, WY</t>
+  </si>
+  <si>
+    <t>Philip Airport, SD</t>
+  </si>
+  <si>
+    <t>Pine Ridge Airport, SD</t>
+  </si>
+  <si>
+    <t>Chadron Airport, NE</t>
+  </si>
+  <si>
+    <t>Moorcroft, WY</t>
+  </si>
+  <si>
+    <t>Faith Airport, SD</t>
+  </si>
+  <si>
+    <t>Gordon Airport, NE</t>
+  </si>
+  <si>
+    <t>Buffalo, SD</t>
+  </si>
+  <si>
+    <t>Gillette  Airport, WY</t>
+  </si>
+  <si>
+    <t>Hettinger Airport, ND</t>
+  </si>
+  <si>
+    <t>Lemmon, SD</t>
+  </si>
+  <si>
+    <t>Lemmon Airport, SD</t>
+  </si>
+  <si>
+    <t>Converse, CO Airport, WY</t>
+  </si>
+  <si>
+    <t>Alliance Airport, NE</t>
+  </si>
+  <si>
+    <t>Douglas, WY</t>
+  </si>
+  <si>
+    <t>Bowman Airport, ND</t>
+  </si>
+  <si>
+    <t>Sibley Peak, WY</t>
+  </si>
+  <si>
+    <t>Pierre Airport, SD</t>
+  </si>
+  <si>
+    <t>Torrington Airport, WY</t>
+  </si>
+  <si>
+    <t>Mission, SD</t>
+  </si>
+  <si>
+    <t>Scottsbluff Airport, NE</t>
+  </si>
+  <si>
+    <t>Miller Field Airport, NE</t>
+  </si>
+  <si>
+    <t>Cheyenne NWS, WY</t>
+  </si>
+  <si>
+    <t>Bismark NWS, ND</t>
+  </si>
+  <si>
+    <t>North Platte NWS, NE</t>
+  </si>
+  <si>
+    <t>Aberdeen NWS, SD</t>
+  </si>
+  <si>
+    <t>Riverton NWS, WY</t>
+  </si>
+  <si>
+    <t>Billings NWS, MT</t>
+  </si>
+  <si>
+    <t>Denver Intl Airport, CO</t>
+  </si>
+  <si>
+    <t>Boulder NWS, CO</t>
+  </si>
+  <si>
+    <t>Sioux Falls NWS, SD</t>
+  </si>
+  <si>
+    <t>Glasgow NWS, MT</t>
+  </si>
+  <si>
+    <t>Goodland NWS KS</t>
+  </si>
+  <si>
+    <t>Hastings NWS, NE</t>
+  </si>
+  <si>
+    <t>Munich School, ND</t>
+  </si>
+  <si>
+    <t>Grand Forks NWS, ND</t>
+  </si>
+  <si>
+    <t>Omaha-Valley NWS, NE</t>
+  </si>
+  <si>
+    <t>Grand Junction NWS, CO</t>
+  </si>
+  <si>
+    <t>Topeka NWS, KS</t>
   </si>
 </sst>
 </file>
@@ -682,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:G47"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -698,7 +711,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -730,7 +743,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="E2">
         <v>44.072699999999998</v>
@@ -747,13 +760,13 @@
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="E3">
         <v>44.133000000000003</v>
@@ -770,13 +783,13 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>44.042999999999999</v>
@@ -793,13 +806,13 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="E5">
         <v>44.133000000000003</v>
@@ -816,13 +829,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="E6">
         <v>43.732999999999997</v>
@@ -839,13 +852,13 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="E7">
         <v>44.482999999999997</v>
@@ -862,13 +875,13 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="E8">
         <v>44.734000000000002</v>
@@ -885,13 +898,13 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="E9">
         <v>44.6629</v>
@@ -908,13 +921,13 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <v>44.051000000000002</v>
@@ -931,13 +944,13 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E11">
         <v>43.021000000000001</v>
@@ -954,13 +967,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="E12">
         <v>42.837000000000003</v>
@@ -977,13 +990,13 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E13">
         <v>44.267000000000003</v>
@@ -1000,13 +1013,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="E14">
         <v>45.031999999999996</v>
@@ -1023,13 +1036,13 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="E15">
         <v>42.805999999999997</v>
@@ -1046,13 +1059,13 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E16">
         <v>45.603999999999999</v>
@@ -1069,13 +1082,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="E17">
         <v>44.338999999999999</v>
@@ -1092,13 +1105,13 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="E18">
         <v>46.014000000000003</v>
@@ -1115,13 +1128,13 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="E19">
         <v>45.933</v>
@@ -1138,13 +1151,13 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E20">
         <v>45.918999999999997</v>
@@ -1161,13 +1174,13 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="E21">
         <v>42.795999999999999</v>
@@ -1184,13 +1197,13 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="E22">
         <v>42.05</v>
@@ -1207,13 +1220,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E23">
         <v>42.75</v>
@@ -1230,13 +1243,13 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="E24">
         <v>46.165500000000002</v>
@@ -1253,13 +1266,13 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="E25">
         <v>42.433</v>
@@ -1276,13 +1289,13 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="E26">
         <v>44.381</v>
@@ -1299,13 +1312,13 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E27">
         <v>42.061</v>
@@ -1322,13 +1335,13 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E28">
         <v>43.033000000000001</v>
@@ -1345,13 +1358,13 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E29">
         <v>41.871000000000002</v>
@@ -1368,13 +1381,13 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E30">
         <v>42.878</v>
@@ -1391,13 +1404,13 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E31">
         <v>41.1556</v>
@@ -1414,13 +1427,13 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="E32">
         <v>46.7727</v>
@@ -1437,13 +1450,13 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="E33">
         <v>41.126199999999997</v>
@@ -1460,13 +1473,13 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E34">
         <v>45.4467</v>
@@ -1483,13 +1496,13 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E35">
         <v>43.0642</v>
@@ -1506,13 +1519,13 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="E36">
         <v>45.7502</v>
@@ -1529,13 +1542,13 @@
         <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E37">
         <v>39.861699999999999</v>
@@ -1552,13 +1565,13 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E38">
         <v>39.991999999999997</v>
@@ -1575,13 +1588,13 @@
         <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E39">
         <v>43.582000000000001</v>
@@ -1598,13 +1611,13 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E40">
         <v>48.212400000000002</v>
@@ -1621,13 +1634,13 @@
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E41">
         <v>39.370699999999999</v>
@@ -1644,13 +1657,13 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E42">
         <v>40.647500000000001</v>
@@ -1667,13 +1680,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E43">
         <v>48.667499999999997</v>
@@ -1690,13 +1703,13 @@
         <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E44">
         <v>47.921900000000001</v>
@@ -1713,13 +1726,13 @@
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E45">
         <v>41.319699999999997</v>
@@ -1736,13 +1749,13 @@
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E46">
         <v>39.122399999999999</v>
@@ -1759,13 +1772,13 @@
         <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E47">
         <v>39.068800000000003</v>

</xml_diff>